<commit_message>
now deployed on railway
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13212"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="252">
   <si>
     <t>First Name</t>
   </si>
@@ -772,6 +772,9 @@
   </si>
   <si>
     <t>Anchal Jain</t>
+  </si>
+  <si>
+    <t>Aryan</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B287"/>
+  <dimension ref="A1:B289"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="B288" sqref="B288"/>
+      <selection activeCell="C289" sqref="C289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3447,6 +3450,22 @@
         <v>8923825140</v>
       </c>
     </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>37</v>
+      </c>
+      <c r="B288">
+        <v>8450956615</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>251</v>
+      </c>
+      <c r="B289">
+        <v>7020120468</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>